<commit_message>
add minor changes to excel
</commit_message>
<xml_diff>
--- a/ExcelProjects/Formula Excel Template.xlsx
+++ b/ExcelProjects/Formula Excel Template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f913f00fe774003/Documents/Data-Analyst/ExcelProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2A1336-4D06-43B4-A5CB-3A8EBDF83F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{FE2A1336-4D06-43B4-A5CB-3A8EBDF83F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70197002-18A0-47C8-A08F-778222AEEBC5}"/>
   <bookViews>
-    <workbookView xWindow="-16956" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
+    <workbookView xWindow="-16956" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="IF-IFS" sheetId="8" r:id="rId1"/>
     <sheet name="Len" sheetId="2" r:id="rId2"/>
-    <sheet name="LeftRight" sheetId="4" r:id="rId3"/>
-    <sheet name="DateToText" sheetId="3" r:id="rId4"/>
+    <sheet name="DateToText" sheetId="3" r:id="rId3"/>
+    <sheet name="LeftRight" sheetId="4" r:id="rId4"/>
     <sheet name="Substitute" sheetId="7" r:id="rId5"/>
     <sheet name="TRIM" sheetId="6" r:id="rId6"/>
     <sheet name="SUM-SumIF" sheetId="12" r:id="rId7"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="91">
   <si>
     <t>FirstName</t>
   </si>
@@ -335,7 +335,10 @@
     <t>Right (year)</t>
   </si>
   <si>
-    <t>=LEFT(J2#,2)</t>
+    <t>day</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -2062,6 +2065,417 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C4862C-FF60-4E24-9054-4C595B8DA66E}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>45000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37197</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42253</v>
+      </c>
+      <c r="J2" t="str" cm="1">
+        <f t="array" ref="J2:J10">TEXT(H2:H10, "dd/mm/yyyy")</f>
+        <v>02/11/2001</v>
+      </c>
+      <c r="K2" t="str" cm="1">
+        <f t="array" ref="K2:K10">LEFT(_xlfn.ANCHORARRAY(J2),2)</f>
+        <v>02</v>
+      </c>
+      <c r="L2" t="str" cm="1">
+        <f t="array" ref="L2:L10">RIGHT(_xlfn.ANCHORARRAY(J2),4)</f>
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3">
+        <v>36000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36436</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42287</v>
+      </c>
+      <c r="J3" t="str">
+        <v>03/10/1999</v>
+      </c>
+      <c r="K3" t="str">
+        <v>03</v>
+      </c>
+      <c r="L3" t="str">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>63000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36711</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42986</v>
+      </c>
+      <c r="J4" t="str">
+        <v>04/07/2000</v>
+      </c>
+      <c r="K4" t="str">
+        <v>04</v>
+      </c>
+      <c r="L4" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5">
+        <v>47000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42341</v>
+      </c>
+      <c r="J5" t="str">
+        <v>05/01/2000</v>
+      </c>
+      <c r="K5" t="str">
+        <v>05</v>
+      </c>
+      <c r="L5" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>50000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>37017</v>
+      </c>
+      <c r="I6" s="1">
+        <v>42977</v>
+      </c>
+      <c r="J6" t="str">
+        <v>06/05/2001</v>
+      </c>
+      <c r="K6" t="str">
+        <v>06</v>
+      </c>
+      <c r="L6" t="str">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7">
+        <v>65000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>35040</v>
+      </c>
+      <c r="I7" s="1">
+        <v>41528</v>
+      </c>
+      <c r="J7" t="str">
+        <v>07/12/1995</v>
+      </c>
+      <c r="K7" t="str">
+        <v>07</v>
+      </c>
+      <c r="L7" t="str">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>41000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>37933</v>
+      </c>
+      <c r="I8" s="1">
+        <v>41551</v>
+      </c>
+      <c r="J8" t="str">
+        <v>08/11/2003</v>
+      </c>
+      <c r="K8" t="str">
+        <v>08</v>
+      </c>
+      <c r="L8" t="str">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>48000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>37416</v>
+      </c>
+      <c r="I9" s="1">
+        <v>42116</v>
+      </c>
+      <c r="J9" t="str">
+        <v>09/06/2002</v>
+      </c>
+      <c r="K9" t="str">
+        <v>09</v>
+      </c>
+      <c r="L9" t="str">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>42000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>37843</v>
+      </c>
+      <c r="I10" s="1">
+        <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <v>10/08/2003</v>
+      </c>
+      <c r="K10" t="str">
+        <v>10</v>
+      </c>
+      <c r="L10" t="str">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC954FE-DA24-43B2-AD9D-17E8CC017065}">
   <sheetPr>
     <tabColor theme="9"/>
@@ -2496,422 +2910,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C4862C-FF60-4E24-9054-4C595B8DA66E}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:M13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>45000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>37197</v>
-      </c>
-      <c r="I2" s="1">
-        <v>42253</v>
-      </c>
-      <c r="J2" t="str" cm="1">
-        <f t="array" ref="J2:J10">TEXT(H2:H10, "dd/mm/yyyy")</f>
-        <v>02/11/2001</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" t="str" cm="1">
-        <f t="array" ref="L2:L10">TEXT(J2:J10, "dd/mm/yyyy")</f>
-        <v>02/11/2001</v>
-      </c>
-      <c r="M2" t="str" cm="1">
-        <f t="array" ref="M2:M10">RIGHT(_xlfn.ANCHORARRAY(L2),4)</f>
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3">
-        <v>36000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>36436</v>
-      </c>
-      <c r="I3" s="1">
-        <v>42287</v>
-      </c>
-      <c r="J3" t="str">
-        <v>03/10/1999</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" t="str">
-        <v>03/10/1999</v>
-      </c>
-      <c r="M3" t="str">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <v>63000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>36711</v>
-      </c>
-      <c r="I4" s="1">
-        <v>42986</v>
-      </c>
-      <c r="J4" t="str">
-        <v>04/07/2000</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" t="str">
-        <v>04/07/2000</v>
-      </c>
-      <c r="M4" t="str">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5">
-        <v>47000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>36530</v>
-      </c>
-      <c r="I5" s="1">
-        <v>42341</v>
-      </c>
-      <c r="J5" t="str">
-        <v>05/01/2000</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" t="str">
-        <v>05/01/2000</v>
-      </c>
-      <c r="M5" t="str">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>50000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>37017</v>
-      </c>
-      <c r="I6" s="1">
-        <v>42977</v>
-      </c>
-      <c r="J6" t="str">
-        <v>06/05/2001</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" t="str">
-        <v>06/05/2001</v>
-      </c>
-      <c r="M6" t="str">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1006</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7">
-        <v>65000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>35040</v>
-      </c>
-      <c r="I7" s="1">
-        <v>41528</v>
-      </c>
-      <c r="J7" t="str">
-        <v>07/12/1995</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" t="str">
-        <v>07/12/1995</v>
-      </c>
-      <c r="M7" t="str">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1007</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>41000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>37933</v>
-      </c>
-      <c r="I8" s="1">
-        <v>41551</v>
-      </c>
-      <c r="J8" t="str">
-        <v>08/11/2003</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" t="str">
-        <v>08/11/2003</v>
-      </c>
-      <c r="M8" t="str">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1008</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>48000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>37416</v>
-      </c>
-      <c r="I9" s="1">
-        <v>42116</v>
-      </c>
-      <c r="J9" t="str">
-        <v>09/06/2002</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" t="str">
-        <v>09/06/2002</v>
-      </c>
-      <c r="M9" t="str">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1009</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>42000</v>
-      </c>
-      <c r="H10" s="1">
-        <v>37843</v>
-      </c>
-      <c r="I10" s="1">
-        <v>40800</v>
-      </c>
-      <c r="J10" t="str">
-        <v>10/08/2003</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" t="str">
-        <v>10/08/2003</v>
-      </c>
-      <c r="M10" t="str">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H13" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B9C42-087D-43BC-95CC-49AE54CDC17A}">
   <sheetPr>
@@ -2919,7 +2917,7 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish with simple excel formulas
</commit_message>
<xml_diff>
--- a/ExcelProjects/Formula Excel Template.xlsx
+++ b/ExcelProjects/Formula Excel Template.xlsx
@@ -8,23 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f913f00fe774003/Documents/Data-Analyst/ExcelProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{FE2A1336-4D06-43B4-A5CB-3A8EBDF83F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70197002-18A0-47C8-A08F-778222AEEBC5}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{FE2A1336-4D06-43B4-A5CB-3A8EBDF83F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9FE7ACE-1AD5-44D0-A867-595804B85DB4}"/>
   <bookViews>
-    <workbookView xWindow="-16956" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
+    <workbookView xWindow="-16956" yWindow="12852" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="9" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="IF-IFS" sheetId="8" r:id="rId1"/>
     <sheet name="Len" sheetId="2" r:id="rId2"/>
     <sheet name="DateToText" sheetId="3" r:id="rId3"/>
     <sheet name="LeftRight" sheetId="4" r:id="rId4"/>
-    <sheet name="Substitute" sheetId="7" r:id="rId5"/>
-    <sheet name="TRIM" sheetId="6" r:id="rId6"/>
-    <sheet name="SUM-SumIF" sheetId="12" r:id="rId7"/>
-    <sheet name="Count-CountIF" sheetId="5" r:id="rId8"/>
-    <sheet name="Concatenate" sheetId="1" r:id="rId9"/>
+    <sheet name="TRIM" sheetId="6" r:id="rId5"/>
+    <sheet name="Concatenate" sheetId="1" r:id="rId6"/>
+    <sheet name="Substitute" sheetId="7" r:id="rId7"/>
+    <sheet name="SUM-SumIF" sheetId="12" r:id="rId8"/>
+    <sheet name="Count-CountIF" sheetId="5" r:id="rId9"/>
     <sheet name="Days-NetworkDays" sheetId="13" r:id="rId10"/>
     <sheet name="Max-Min" sheetId="9" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Days-NetworkDays'!$H$2:$H$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -66,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="98">
   <si>
     <t>FirstName</t>
   </si>
@@ -122,9 +125,6 @@
     <t>Hudson</t>
   </si>
   <si>
-    <t>CONCATENATE(B2," ",C2)</t>
-  </si>
-  <si>
     <t>LEN(B2)</t>
   </si>
   <si>
@@ -284,9 +284,6 @@
     <t>with 1 instance</t>
   </si>
   <si>
-    <t>with 2 instances</t>
-  </si>
-  <si>
     <t>with NO instances</t>
   </si>
   <si>
@@ -339,13 +336,41 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>EMail</t>
+  </si>
+  <si>
+    <t>CONCAT(B2," ",C2)</t>
+  </si>
+  <si>
+    <t>5-6-2001</t>
+  </si>
+  <si>
+    <t>9-11-2013</t>
+  </si>
+  <si>
+    <t>1.5.2000</t>
+  </si>
+  <si>
+    <t>12.3.2015</t>
+  </si>
+  <si>
+    <t>with 2 instance</t>
+  </si>
+  <si>
+    <t>the  format change:</t>
+  </si>
+  <si>
+    <t>#value error in Days function (it's because your system date format doesn't match the given one). 
+Select all dates (h2:h10) -&gt; go to Data tab -&gt; choose Text to Columns from there -&gt; Delimited, Next-&gt;, Next -&gt;, step 3 of 3: column date format and chose DMY -&gt; finish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +380,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Abadi"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -380,10 +419,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,7 +760,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -725,28 +769,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -763,10 +807,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -800,10 +844,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -835,10 +879,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -870,10 +914,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -905,10 +949,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -940,10 +984,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -966,19 +1010,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -1010,10 +1054,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -1045,10 +1089,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -1076,21 +1120,23 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1099,28 +1145,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1137,19 +1183,27 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>45000</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>56</v>
+      <c r="H2" s="1">
+        <v>37197</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42253</v>
+      </c>
+      <c r="J2" s="3" cm="1">
+        <f t="array" ref="J2:J10">_xlfn.DAYS(I2:I10,H2:H10)</f>
+        <v>5056</v>
+      </c>
+      <c r="K2">
+        <f>NETWORKDAYS(H2,I2)</f>
+        <v>3611</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1166,19 +1220,26 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>36000</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>57</v>
+      <c r="H3" s="1">
+        <v>36436</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42287</v>
+      </c>
+      <c r="J3">
+        <v>5851</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="0">NETWORKDAYS(H3,I3)</f>
+        <v>4180</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1195,19 +1256,26 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>63000</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>58</v>
+      <c r="H4" s="1">
+        <v>36711</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42986</v>
+      </c>
+      <c r="J4">
+        <v>6275</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>4484</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1224,19 +1292,26 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>47000</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>59</v>
+      <c r="H5" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42341</v>
+      </c>
+      <c r="J5">
+        <v>5811</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>4152</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1253,19 +1328,26 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>50000</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>60</v>
+      <c r="H6" s="1">
+        <v>37017</v>
+      </c>
+      <c r="I6" s="1">
+        <v>42977</v>
+      </c>
+      <c r="J6">
+        <v>5960</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>4258</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1282,19 +1364,26 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>65000</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>61</v>
+      <c r="H7" s="1">
+        <v>37017</v>
+      </c>
+      <c r="I7" s="1">
+        <v>41528</v>
+      </c>
+      <c r="J7">
+        <v>4511</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>3223</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1302,28 +1391,35 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>41000</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>61</v>
+      <c r="H8" s="1">
+        <v>37933</v>
+      </c>
+      <c r="I8" s="1">
+        <v>41528</v>
+      </c>
+      <c r="J8">
+        <v>3595</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>2568</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1340,19 +1436,26 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>48000</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>62</v>
+      <c r="H9" s="1">
+        <v>37416</v>
+      </c>
+      <c r="I9" s="1">
+        <v>42116</v>
+      </c>
+      <c r="J9">
+        <v>4700</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>3358</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1369,22 +1472,99 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>42000</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="H10" s="1">
+        <v>37843</v>
+      </c>
+      <c r="I10" s="1">
+        <v>42116</v>
+      </c>
+      <c r="J10">
+        <v>4273</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:J17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1408,7 +1588,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1417,28 +1597,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1455,10 +1635,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -1492,10 +1672,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -1525,10 +1705,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -1554,10 +1734,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -1583,10 +1763,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -1612,10 +1792,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -1632,19 +1812,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -1670,10 +1850,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -1699,10 +1879,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -1737,7 +1917,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1746,28 +1926,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1784,10 +1964,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -1817,10 +1997,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -1849,10 +2029,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -1881,10 +2061,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -1913,10 +2093,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -1945,10 +2125,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -1968,19 +2148,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -2009,10 +2189,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -2041,10 +2221,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -2072,7 +2252,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2263,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2092,31 +2272,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2133,10 +2313,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -2174,10 +2354,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -2212,10 +2392,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -2250,10 +2430,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -2288,10 +2468,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -2326,10 +2506,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -2355,19 +2535,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -2402,10 +2582,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -2440,10 +2620,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -2494,7 +2674,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2503,34 +2683,34 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
-        <v>38</v>
-      </c>
       <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" t="s">
         <v>86</v>
-      </c>
-      <c r="L1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2547,22 +2727,22 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>45000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" t="str" cm="1">
         <f t="array" ref="K2:K10">LEFT(B2:B10,3)</f>
@@ -2591,22 +2771,22 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>36000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K3" t="str">
         <v>Pam</v>
@@ -2632,22 +2812,22 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>63000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K4" t="str">
         <v>Dwi</v>
@@ -2673,22 +2853,22 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>47000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" t="str">
         <v>Ang</v>
@@ -2714,22 +2894,22 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>50000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" t="str">
         <v>Tob</v>
@@ -2755,22 +2935,22 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>65000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" t="str">
         <v>Mic</v>
@@ -2787,31 +2967,31 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>41000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K8" t="str">
         <v>Mer</v>
@@ -2837,22 +3017,22 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>48000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K9" t="str">
         <v>Sta</v>
@@ -2878,22 +3058,22 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>42000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K10" t="str">
         <v>Kev</v>
@@ -2911,14 +3091,1540 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F69BBA-836F-48E1-B067-27B71B706556}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>45000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37197</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42253</v>
+      </c>
+      <c r="J2" t="str" cm="1">
+        <f t="array" ref="J2:J10">TRIM(C2:C10)</f>
+        <v>Halpert</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>36000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36436</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42287</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Beasley</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>63000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36711</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42986</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Schrute</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>47000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42341</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Martin</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>50000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>37017</v>
+      </c>
+      <c r="I6" s="1">
+        <v>42977</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Flenderson</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>65000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>35040</v>
+      </c>
+      <c r="I7" s="1">
+        <v>41528</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Scott</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>41000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>37933</v>
+      </c>
+      <c r="I8" s="1">
+        <v>41551</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Palmer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>48000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>37416</v>
+      </c>
+      <c r="I9" s="1">
+        <v>42116</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Hudson</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>42000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>37843</v>
+      </c>
+      <c r="I10" s="1">
+        <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Malone</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB977C31-5FD1-4473-A6A1-29ABAD3F7755}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>45000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37197</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42253</v>
+      </c>
+      <c r="J2" t="str">
+        <f>_xlfn.CONCAT(B2, " ",C2)</f>
+        <v>Jim Halpert</v>
+      </c>
+      <c r="K2" t="str">
+        <f>_xlfn.CONCAT(B2,".",C2,"@colournika.ca")</f>
+        <v>Jim.Halpert@colournika.ca</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>36000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36436</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42287</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">_xlfn.CONCAT(B3, " ",C3)</f>
+        <v>Pam Beasley</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K10" si="1">_xlfn.CONCAT(B3,".",C3,"@colournika.ca")</f>
+        <v>Pam.Beasley@colournika.ca</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>63000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36711</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42986</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Dwight Schrute</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>Dwight.Schrute@colournika.ca</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>47000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42341</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Angela Martin</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>Angela.Martin@colournika.ca</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>50000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>37017</v>
+      </c>
+      <c r="I6" s="1">
+        <v>42977</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Toby Flenderson</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>Toby.Flenderson@colournika.ca</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>65000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>35040</v>
+      </c>
+      <c r="I7" s="1">
+        <v>41528</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael Scott</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>Michael.Scott@colournika.ca</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>41000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>37933</v>
+      </c>
+      <c r="I8" s="1">
+        <v>41551</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Meredith Palmer</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>Meredith.Palmer@colournika.ca</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>48000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>37416</v>
+      </c>
+      <c r="I9" s="1">
+        <v>42116</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Stanley Hudson</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>Stanley.Hudson@colournika.ca</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>42000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>37843</v>
+      </c>
+      <c r="I10" s="1">
+        <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Kevin Malone</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>Kevin.Malone@colournika.ca</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <f t="shared" ref="H11:H12" si="2">CONCATENATE(B11," ",C11)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B9C42-087D-43BC-95CC-49AE54CDC17A}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>45000</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="str" cm="1">
+        <f t="array" ref="J2:J10">SUBSTITUTE(SUBSTITUTE(H2:H10, ".", "/"), "-","/")</f>
+        <v>11/2/2001</v>
+      </c>
+      <c r="K2" t="str" cm="1">
+        <f t="array" ref="K2:K10">SUBSTITUTE(_xlfn.ANCHORARRAY(J2),"/", "-",1)</f>
+        <v>11-2/2001</v>
+      </c>
+      <c r="L2" t="str" cm="1">
+        <f t="array" ref="L2:L10">SUBSTITUTE(_xlfn.ANCHORARRAY(J2),"/", "-",2)</f>
+        <v>11/2-2001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>36000</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="str">
+        <v>10/3/1999</v>
+      </c>
+      <c r="K3" t="str">
+        <v>10-3/1999</v>
+      </c>
+      <c r="L3" t="str">
+        <v>10/3-1999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>63000</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" t="str">
+        <v>7/4/2000</v>
+      </c>
+      <c r="K4" t="str">
+        <v>7-4/2000</v>
+      </c>
+      <c r="L4" t="str">
+        <v>7/4-2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>47000</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" t="str">
+        <v>1/5/2000</v>
+      </c>
+      <c r="K5" t="str">
+        <v>1-5/2000</v>
+      </c>
+      <c r="L5" t="str">
+        <v>1/5-2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>50000</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="str">
+        <v>5/6/2001</v>
+      </c>
+      <c r="K6" t="str">
+        <v>5-6/2001</v>
+      </c>
+      <c r="L6" t="str">
+        <v>5/6-2001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>65000</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" t="str">
+        <v>5/6/2001</v>
+      </c>
+      <c r="K7" t="str">
+        <v>5-6/2001</v>
+      </c>
+      <c r="L7" t="str">
+        <v>5/6-2001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>41000</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="str">
+        <v>11/8/2003</v>
+      </c>
+      <c r="K8" t="str">
+        <v>11-8/2003</v>
+      </c>
+      <c r="L8" t="str">
+        <v>11/8-2003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>48000</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="str">
+        <v>6/9/2002</v>
+      </c>
+      <c r="K9" t="str">
+        <v>6-9/2002</v>
+      </c>
+      <c r="L9" t="str">
+        <v>6/9-2002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>42000</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="str">
+        <v>8/10/2003</v>
+      </c>
+      <c r="K10" t="str">
+        <v>8-10/2003</v>
+      </c>
+      <c r="L10" t="str">
+        <v>8/10-2003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D41C5D0-EC67-4288-8B29-30C6E5CFEE73}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>45000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37197</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42253</v>
+      </c>
+      <c r="J2">
+        <f>SUM(G2:G10)</f>
+        <v>437000</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(G2:G10, "&gt;50000")</f>
+        <v>128000</v>
+      </c>
+      <c r="L2">
+        <f>SUMIFS(G2:G10, E2:E10,"Female", D2:D10, "&gt;30")</f>
+        <v>88000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>36000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36436</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>63000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36711</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42986</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>47000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>50000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>37017</v>
+      </c>
+      <c r="I6" s="1">
+        <v>42977</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>65000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>35040</v>
+      </c>
+      <c r="I7" s="1">
+        <v>41528</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>41000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>37933</v>
+      </c>
+      <c r="I8" s="1">
+        <v>41551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>48000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>37416</v>
+      </c>
+      <c r="I9" s="1">
+        <v>42116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>42000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>37843</v>
+      </c>
+      <c r="I10" s="1">
+        <v>40800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D217F6E-9452-40AF-AFA2-377600A25F44}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2929,7 +4635,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2938,31 +4644,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2979,19 +4685,31 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>45000</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>56</v>
+      <c r="H2" s="1">
+        <v>37197</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42253</v>
+      </c>
+      <c r="J2">
+        <f>COUNT(A2:A10)</f>
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(G2:G10, "&gt;45000")</f>
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIFS(A2:A10, "&gt;1005", E2:E10, "Male")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3008,19 +4726,19 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3">
         <v>36000</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>57</v>
+      <c r="H3" s="1">
+        <v>36436</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42287</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3037,19 +4755,19 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4">
         <v>63000</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>58</v>
+      <c r="H4" s="1">
+        <v>36711</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42986</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3066,19 +4784,19 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5">
         <v>47000</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>59</v>
+      <c r="H5" s="1">
+        <v>36530</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42341</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3095,19 +4813,19 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>50000</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>60</v>
+      <c r="H6" s="1">
+        <v>37017</v>
+      </c>
+      <c r="I6" s="1">
+        <v>42977</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3124,19 +4842,19 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>65000</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>61</v>
+      <c r="H7" s="1">
+        <v>35040</v>
+      </c>
+      <c r="I7" s="1">
+        <v>41528</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3144,28 +4862,28 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>41000</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>61</v>
+      <c r="H8" s="1">
+        <v>37933</v>
+      </c>
+      <c r="I8" s="1">
+        <v>41551</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3182,19 +4900,19 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>48000</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>62</v>
+      <c r="H9" s="1">
+        <v>37416</v>
+      </c>
+      <c r="I9" s="1">
+        <v>42116</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3211,1343 +4929,19 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>42000</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F69BBA-836F-48E1-B067-27B71B706556}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>45000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>37197</v>
-      </c>
-      <c r="I2" s="1">
-        <v>42253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3">
-        <v>36000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>36436</v>
-      </c>
-      <c r="I3" s="1">
-        <v>42287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <v>63000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>36711</v>
-      </c>
-      <c r="I4" s="1">
-        <v>42986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1004</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5">
-        <v>47000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>36530</v>
-      </c>
-      <c r="I5" s="1">
-        <v>42341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1005</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>50000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>37017</v>
-      </c>
-      <c r="I6" s="1">
-        <v>42977</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1006</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7">
-        <v>65000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>35040</v>
-      </c>
-      <c r="I7" s="1">
-        <v>41528</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1007</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>41000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>37933</v>
-      </c>
-      <c r="I8" s="1">
-        <v>41551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1008</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>48000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>37416</v>
-      </c>
-      <c r="I9" s="1">
-        <v>42116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1009</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>42000</v>
-      </c>
       <c r="H10" s="1">
         <v>37843</v>
       </c>
       <c r="I10" s="1">
         <v>40800</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D41C5D0-EC67-4288-8B29-30C6E5CFEE73}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:L10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>45000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>37197</v>
-      </c>
-      <c r="I2" s="1">
-        <v>42253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3">
-        <v>36000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>36436</v>
-      </c>
-      <c r="I3" s="1">
-        <v>42287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <v>63000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>36711</v>
-      </c>
-      <c r="I4" s="1">
-        <v>42986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5">
-        <v>47000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>36530</v>
-      </c>
-      <c r="I5" s="1">
-        <v>42341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>50000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>37017</v>
-      </c>
-      <c r="I6" s="1">
-        <v>42977</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1006</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7">
-        <v>65000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>35040</v>
-      </c>
-      <c r="I7" s="1">
-        <v>41528</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1007</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>41000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>37933</v>
-      </c>
-      <c r="I8" s="1">
-        <v>41551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1008</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>48000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>37416</v>
-      </c>
-      <c r="I9" s="1">
-        <v>42116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1009</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>42000</v>
-      </c>
-      <c r="H10" s="1">
-        <v>37843</v>
-      </c>
-      <c r="I10" s="1">
-        <v>40800</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D217F6E-9452-40AF-AFA2-377600A25F44}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:L10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>45000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>37197</v>
-      </c>
-      <c r="I2" s="1">
-        <v>42253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3">
-        <v>36000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>36436</v>
-      </c>
-      <c r="I3" s="1">
-        <v>42287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <v>63000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>36711</v>
-      </c>
-      <c r="I4" s="1">
-        <v>42986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5">
-        <v>47000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>36530</v>
-      </c>
-      <c r="I5" s="1">
-        <v>42341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>50000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>37017</v>
-      </c>
-      <c r="I6" s="1">
-        <v>42977</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1006</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7">
-        <v>65000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>35040</v>
-      </c>
-      <c r="I7" s="1">
-        <v>41528</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1007</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>41000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>37933</v>
-      </c>
-      <c r="I8" s="1">
-        <v>41551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1008</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>48000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>37416</v>
-      </c>
-      <c r="I9" s="1">
-        <v>42116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1009</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>42000</v>
-      </c>
-      <c r="H10" s="1">
-        <v>37843</v>
-      </c>
-      <c r="I10" s="1">
-        <v>40800</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB977C31-5FD1-4473-A6A1-29ABAD3F7755}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:J12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>45000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>37197</v>
-      </c>
-      <c r="I2" s="1">
-        <v>42253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3">
-        <v>36000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>36436</v>
-      </c>
-      <c r="I3" s="1">
-        <v>42287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4">
-        <v>63000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>36711</v>
-      </c>
-      <c r="I4" s="1">
-        <v>42986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5">
-        <v>47000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>36530</v>
-      </c>
-      <c r="I5" s="1">
-        <v>42341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>50000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>37017</v>
-      </c>
-      <c r="I6" s="1">
-        <v>42977</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1006</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7">
-        <v>65000</v>
-      </c>
-      <c r="H7" s="1">
-        <v>35040</v>
-      </c>
-      <c r="I7" s="1">
-        <v>41528</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1007</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>41000</v>
-      </c>
-      <c r="H8" s="1">
-        <v>37933</v>
-      </c>
-      <c r="I8" s="1">
-        <v>41551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1008</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>48000</v>
-      </c>
-      <c r="H9" s="1">
-        <v>37416</v>
-      </c>
-      <c r="I9" s="1">
-        <v>42116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1009</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>42000</v>
-      </c>
-      <c r="H10" s="1">
-        <v>37843</v>
-      </c>
-      <c r="I10" s="1">
-        <v>40800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H11" t="str">
-        <f t="shared" ref="H11:H12" si="0">CONCATENATE(B11," ",C11)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
       </c>
     </row>
   </sheetData>

</xml_diff>